<commit_message>
update đơn mua + import excel
</commit_message>
<xml_diff>
--- a/BE-DATN-SD47/test - Copy - Copy.xlsx
+++ b/BE-DATN-SD47/test - Copy - Copy.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATN-SD47\BE-DATN-SD47\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D5108D3-94EE-4E5B-ADF8-56DB4D0DC3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8B9B9F-90C0-40EB-8F57-142FC25F60D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E7871901-05C9-4966-B7A1-8DCFE58BD91A}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -58,7 +58,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -68,7 +67,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,16 +78,6 @@
       <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="none">
-        <fgColor indexed="13"/>
       </patternFill>
     </fill>
   </fills>
@@ -104,11 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,13 +413,13 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="1" width="25.33203125" collapsed="true"/>
-    <col min="2" max="16384" style="1" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="25.33203125" style="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -476,22 +463,22 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
+      <c r="A3" s="1">
         <v>1.2312312312312301E+17</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="1">
         <v>41</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="1">
         <v>9</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="1">
         <v>399999</v>
       </c>
     </row>
@@ -512,7 +499,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="1">
-        <v>399999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -529,29 +516,29 @@
         <v>2</v>
       </c>
       <c r="E5" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F5" s="1">
         <v>399999</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>38</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>9</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>499999</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update hoàn trả + detail hóa đơn
</commit_message>
<xml_diff>
--- a/BE-DATN-SD47/test - Copy - Copy.xlsx
+++ b/BE-DATN-SD47/test - Copy - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATN-SD47\BE-DATN-SD47\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8B9B9F-90C0-40EB-8F57-142FC25F60D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F78ABB-76ED-4BFC-B963-62E8748FC923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E7871901-05C9-4966-B7A1-8DCFE58BD91A}"/>
   </bookViews>
@@ -413,13 +413,15 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="25.33203125" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="16384" width="8.88671875" style="1" collapsed="1"/>
+    <col min="2" max="5" width="8.88671875" style="1" collapsed="1"/>
+    <col min="6" max="6" width="11" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -499,7 +501,7 @@
         <v>15</v>
       </c>
       <c r="F4" s="1">
-        <v>0</v>
+        <v>1000000000</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -516,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="1">
-        <v>0</v>
+        <v>9999</v>
       </c>
       <c r="F5" s="1">
         <v>399999</v>

</xml_diff>